<commit_message>
paar dingen in moscow vergeten
</commit_message>
<xml_diff>
--- a/Tijdelijke map documenten/MoSCoW Planning.xlsx
+++ b/Tijdelijke map documenten/MoSCoW Planning.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_GoBack" localSheetId="0">Sheet1!$A$26</definedName>
+  </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Taak</t>
   </si>
@@ -142,15 +145,34 @@
   </si>
   <si>
     <t>besturing tests uitvoeren</t>
+  </si>
+  <si>
+    <t>wasmachine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Het uitvoeren van verschillende was programma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Logs bijhouden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Noodknop.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -254,6 +276,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -307,126 +337,129 @@
   </borders>
   <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="15" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -827,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q1048573"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1199,82 +1232,90 @@
       <c r="L24" s="19"/>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
+      <c r="A25" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
       <c r="I25" s="7"/>
       <c r="L25" s="29"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="9" t="s">
-        <v>40</v>
+      <c r="A26" s="34" t="s">
+        <v>42</v>
       </c>
       <c r="C26" s="33"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="I26" s="7"/>
       <c r="L26" s="29"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="A27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
+      <c r="A27" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="36"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
       <c r="I27" s="7"/>
       <c r="K27" s="15"/>
       <c r="L27" s="29"/>
     </row>
     <row r="28" spans="1:17">
-      <c r="A28" s="9" t="s">
-        <v>19</v>
+      <c r="A28" s="34" t="s">
+        <v>44</v>
       </c>
       <c r="C28" s="33"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:17">
-      <c r="A29" s="4"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+      <c r="A29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
       <c r="I29" s="7"/>
       <c r="L29" s="28"/>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="5"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
+      <c r="A30" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="33"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
       <c r="I30" s="7"/>
       <c r="L30" s="28"/>
     </row>
     <row r="31" spans="1:17">
-      <c r="A31" s="5"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
+      <c r="A31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="33"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
       <c r="I31" s="7"/>
       <c r="L31" s="28"/>
     </row>
     <row r="32" spans="1:17">
-      <c r="A32" s="5"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
+      <c r="A32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="33"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:12">

</xml_diff>